<commit_message>
impl excel reader with ignore hidden rows option
</commit_message>
<xml_diff>
--- a/resource/testData/compined_data.xlsx
+++ b/resource/testData/compined_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\cSharp\Crab-Excel-Data-App\resource\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63FB15CA-1F8C-420A-8119-CEB463D58AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2F14680-FBB5-40C7-92F5-5554FE1CCAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3435" windowWidth="11985" windowHeight="11295" xr2:uid="{FC8BC938-FECA-4939-BBF0-A61B72140D71}"/>
+    <workbookView xWindow="3000" yWindow="3435" windowWidth="11985" windowHeight="11295" xr2:uid="{03371D2C-8D55-4149-A349-3B3B0125F0A1}"/>
   </bookViews>
   <sheets>
     <sheet name="total_data" sheetId="2" r:id="rId1"/>
@@ -686,7 +686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13400BBD-F4CF-4366-94CC-1222FB0F22CC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3761DF11-6C02-4B67-B676-7394E6C25B48}">
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1133,7 +1133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC60CDB5-1D08-46E6-BCD2-C9E85A5983EA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C86A8992-19C2-4EC2-A20C-350EF079F2E9}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
add checkbox for ignore hidden rows
</commit_message>
<xml_diff>
--- a/resource/testData/compined_data.xlsx
+++ b/resource/testData/compined_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\cSharp\Crab-Excel-Data-App\resource\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2F14680-FBB5-40C7-92F5-5554FE1CCAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F58A739D-7DA4-4A8A-9798-2EBB80025EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3435" windowWidth="11985" windowHeight="11295" xr2:uid="{03371D2C-8D55-4149-A349-3B3B0125F0A1}"/>
+    <workbookView xWindow="3000" yWindow="3435" windowWidth="11985" windowHeight="11295" xr2:uid="{2523A4F4-6AA3-4D78-BF54-BCFA0EC79786}"/>
   </bookViews>
   <sheets>
     <sheet name="total_data" sheetId="2" r:id="rId1"/>
@@ -686,7 +686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3761DF11-6C02-4B67-B676-7394E6C25B48}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B0E554-9CB5-4ABE-9E2E-165465676DFD}">
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1133,7 +1133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C86A8992-19C2-4EC2-A20C-350EF079F2E9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B08F3E5-F8D5-4B0F-9628-95C80B9D260C}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
[dev] save works: find first value cell
</commit_message>
<xml_diff>
--- a/resource/testData/compined_data.xlsx
+++ b/resource/testData/compined_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\cSharp\Crab-Excel-Data-App\resource\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F58A739D-7DA4-4A8A-9798-2EBB80025EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{42F67988-1DA9-46F6-A44D-678B28DADA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3435" windowWidth="11985" windowHeight="11295" xr2:uid="{2523A4F4-6AA3-4D78-BF54-BCFA0EC79786}"/>
+    <workbookView xWindow="3000" yWindow="3435" windowWidth="11985" windowHeight="11295" xr2:uid="{F605B6A4-021E-47E1-A78C-72E0CB13BD3D}"/>
   </bookViews>
   <sheets>
     <sheet name="total_data" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="106">
   <si>
     <t>ID</t>
   </si>
@@ -185,6 +185,24 @@
   </si>
   <si>
     <t>White</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>Nod</t>
+  </si>
+  <si>
+    <t>Rod</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>Mori</t>
+  </si>
+  <si>
+    <t>Cox</t>
   </si>
   <si>
     <t>14</t>
@@ -686,8 +704,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B0E554-9CB5-4ABE-9E2E-165465676DFD}">
-  <dimension ref="A1:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41EF82BF-7515-4426-88C4-B9584B938BCA}">
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -900,7 +918,7 @@
         <v>52</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -914,63 +932,63 @@
         <v>55</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D18" s="1" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -978,55 +996,55 @@
         <v>68</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="D21" s="1" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="D23" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1040,21 +1058,21 @@
         <v>83</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1068,7 +1086,7 @@
         <v>89</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1082,7 +1100,7 @@
         <v>92</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1093,37 +1111,65 @@
         <v>94</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1133,7 +1179,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B08F3E5-F8D5-4B0F-9628-95C80B9D260C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A84E840-E3B1-4D79-A0E5-30B6D4440CD4}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
impl advantage filter for excel data
</commit_message>
<xml_diff>
--- a/resource/testData/compined_data.xlsx
+++ b/resource/testData/compined_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\cSharp\Crab-Excel-Data-App\resource\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42F67988-1DA9-46F6-A44D-678B28DADA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FD2A215-F2DA-4710-BA2C-7AA060E137F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3435" windowWidth="11985" windowHeight="11295" xr2:uid="{F605B6A4-021E-47E1-A78C-72E0CB13BD3D}"/>
+    <workbookView xWindow="3000" yWindow="3435" windowWidth="11985" windowHeight="11295" xr2:uid="{70B47D85-BAB3-4F9D-9531-BC392E0F925A}"/>
   </bookViews>
   <sheets>
     <sheet name="total_data" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="100">
   <si>
     <t>ID</t>
   </si>
@@ -185,24 +185,6 @@
   </si>
   <si>
     <t>White</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
-  <si>
-    <t>Nod</t>
-  </si>
-  <si>
-    <t>Rod</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>Mori</t>
-  </si>
-  <si>
-    <t>Cox</t>
   </si>
   <si>
     <t>14</t>
@@ -704,8 +686,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41EF82BF-7515-4426-88C4-B9584B938BCA}">
-  <dimension ref="A1:D33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D110BE71-7D8B-478E-8611-3939E6263E60}">
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -918,7 +900,7 @@
         <v>52</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -932,63 +914,63 @@
         <v>55</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="D19" s="1" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -996,55 +978,55 @@
         <v>68</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1058,21 +1040,21 @@
         <v>83</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>84</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1086,7 +1068,7 @@
         <v>89</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1100,7 +1082,7 @@
         <v>92</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1111,65 +1093,37 @@
         <v>94</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>95</v>
+        <v>14</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="D30" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="C31" s="1" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1179,7 +1133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A84E840-E3B1-4D79-A0E5-30B6D4440CD4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED56EEC7-E64A-4D76-90A1-EDA8D941CAC2}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>